<commit_message>
Manual Tecnico 100%, Ficha de Proyecto 90%, Manual de usuario 90% y la demas documentacion 100%
</commit_message>
<xml_diff>
--- a/Documentation/Diccionario de datos.xlsx
+++ b/Documentation/Diccionario de datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APRENDIZSENA\Downloads\Emprendev-SB\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBASTIAN\Downloads\Emprendev-SB\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A0524A-9103-47F4-BEA2-DCBD0B0741AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67DC725-DD24-4DF4-BF32-D49D44491C24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="124">
   <si>
     <t>Nombre</t>
   </si>
@@ -333,24 +333,6 @@
     <t>En este campo el mipyme pondra una foto referente a su oferta</t>
   </si>
   <si>
-    <t>tagsId</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>img</t>
-  </si>
-  <si>
-    <t>En este campo se creara un identificador para cada etiqueta</t>
-  </si>
-  <si>
-    <t>En este campo se guardara el nombre de cada etiqueta</t>
-  </si>
-  <si>
-    <t>En este campo se guardara una imagen que identifique a cada etiqueta</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -385,9 +367,6 @@
   </si>
   <si>
     <t>passwordUpdateDate</t>
-  </si>
-  <si>
-    <t>Tbl_etiquetas</t>
   </si>
   <si>
     <t>Tbl_dev</t>
@@ -833,7 +812,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="95" workbookViewId="0">
-      <selection sqref="A1:G57"/>
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,12 +827,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="E1" s="9" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
@@ -880,7 +859,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -889,13 +868,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -909,13 +888,13 @@
         <v>13</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,13 +908,13 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -948,6 +927,15 @@
       <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -970,11 +958,6 @@
       <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -986,15 +969,11 @@
       <c r="C9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="E9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1006,14 +985,14 @@
       <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>32</v>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1027,13 +1006,13 @@
         <v>54</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1047,13 +1026,13 @@
         <v>8</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1067,13 +1046,13 @@
         <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1109,7 +1088,7 @@
         <v>58</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -1145,13 +1124,13 @@
         <v>12</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1159,34 +1138,43 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="E19" s="4" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="E20" s="4" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
+      <c r="E21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1198,10 +1186,19 @@
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>3</v>
@@ -1209,11 +1206,6 @@
       <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1225,15 +1217,11 @@
       <c r="C24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="E24" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1245,14 +1233,14 @@
       <c r="C25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>18</v>
+      <c r="E25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1266,13 +1254,13 @@
         <v>64</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1286,13 +1274,13 @@
         <v>66</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>112</v>
+        <v>3</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1306,13 +1294,13 @@
         <v>68</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1326,13 +1314,13 @@
         <v>70</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1356,11 +1344,7 @@
       <c r="C31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -1372,17 +1356,8 @@
       <c r="C32" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -1392,55 +1367,15 @@
       <c r="C33" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E34" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
-      <c r="E36" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,9 +1386,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>3</v>
@@ -1461,9 +1396,8 @@
       <c r="C38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>83</v>
       </c>
@@ -1474,7 +1408,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>84</v>
       </c>
@@ -1485,7 +1419,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>85</v>
       </c>
@@ -1496,7 +1430,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>86</v>
       </c>
@@ -1507,14 +1441,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>91</v>
       </c>
@@ -1536,7 +1470,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>92</v>
       </c>
@@ -1547,7 +1481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>93</v>
       </c>
@@ -1658,18 +1592,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E16:G16"/>
     <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="A44:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="29" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="28" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>